<commit_message>
fixed ma and exp smoothing
</commit_message>
<xml_diff>
--- a/hw4/ABC_alpha0.1/generated_spreadsheet.xlsx
+++ b/hw4/ABC_alpha0.1/generated_spreadsheet.xlsx
@@ -4823,62 +4823,62 @@
     </row>
     <row r="62" spans="1:11">
       <c r="D62">
-        <v>9750</v>
+        <v>9416.666666666666</v>
       </c>
     </row>
     <row r="63" spans="1:11">
       <c r="D63">
-        <v>9750</v>
+        <v>9416.666666666666</v>
       </c>
     </row>
     <row r="64" spans="1:11">
       <c r="D64">
-        <v>9750</v>
+        <v>9416.666666666666</v>
       </c>
     </row>
     <row r="65" spans="4:4">
       <c r="D65">
-        <v>9750</v>
+        <v>9416.666666666666</v>
       </c>
     </row>
     <row r="66" spans="4:4">
       <c r="D66">
-        <v>9750</v>
+        <v>9416.666666666666</v>
       </c>
     </row>
     <row r="67" spans="4:4">
       <c r="D67">
-        <v>9750</v>
+        <v>9416.666666666666</v>
       </c>
     </row>
     <row r="68" spans="4:4">
       <c r="D68">
-        <v>9750</v>
+        <v>9416.666666666666</v>
       </c>
     </row>
     <row r="69" spans="4:4">
       <c r="D69">
-        <v>9750</v>
+        <v>9416.666666666666</v>
       </c>
     </row>
     <row r="70" spans="4:4">
       <c r="D70">
-        <v>9750</v>
+        <v>9416.666666666666</v>
       </c>
     </row>
     <row r="71" spans="4:4">
       <c r="D71">
-        <v>9750</v>
+        <v>9416.666666666666</v>
       </c>
     </row>
     <row r="72" spans="4:4">
       <c r="D72">
-        <v>9750</v>
+        <v>9416.666666666666</v>
       </c>
     </row>
     <row r="73" spans="4:4">
       <c r="D73">
-        <v>9750</v>
+        <v>9416.666666666666</v>
       </c>
     </row>
   </sheetData>
@@ -7039,62 +7039,62 @@
     </row>
     <row r="63" spans="1:11">
       <c r="D63">
-        <v>11444.54596090322</v>
+        <v>11100.0913648129</v>
       </c>
     </row>
     <row r="64" spans="1:11">
       <c r="D64">
-        <v>11444.54596090322</v>
+        <v>11100.0913648129</v>
       </c>
     </row>
     <row r="65" spans="4:4">
       <c r="D65">
-        <v>11444.54596090322</v>
+        <v>11100.0913648129</v>
       </c>
     </row>
     <row r="66" spans="4:4">
       <c r="D66">
-        <v>11444.54596090322</v>
+        <v>11100.0913648129</v>
       </c>
     </row>
     <row r="67" spans="4:4">
       <c r="D67">
-        <v>11444.54596090322</v>
+        <v>11100.0913648129</v>
       </c>
     </row>
     <row r="68" spans="4:4">
       <c r="D68">
-        <v>11444.54596090322</v>
+        <v>11100.0913648129</v>
       </c>
     </row>
     <row r="69" spans="4:4">
       <c r="D69">
-        <v>11444.54596090322</v>
+        <v>11100.0913648129</v>
       </c>
     </row>
     <row r="70" spans="4:4">
       <c r="D70">
-        <v>11444.54596090322</v>
+        <v>11100.0913648129</v>
       </c>
     </row>
     <row r="71" spans="4:4">
       <c r="D71">
-        <v>11444.54596090322</v>
+        <v>11100.0913648129</v>
       </c>
     </row>
     <row r="72" spans="4:4">
       <c r="D72">
-        <v>11444.54596090322</v>
+        <v>11100.0913648129</v>
       </c>
     </row>
     <row r="73" spans="4:4">
       <c r="D73">
-        <v>11444.54596090322</v>
+        <v>11100.0913648129</v>
       </c>
     </row>
     <row r="74" spans="4:4">
       <c r="D74">
-        <v>11444.54596090322</v>
+        <v>11100.0913648129</v>
       </c>
     </row>
   </sheetData>
@@ -9572,13 +9572,13 @@
         <v>2000</v>
       </c>
       <c r="C3">
-        <v>5998.537928618207</v>
+        <v>5943.363229779768</v>
       </c>
       <c r="D3">
-        <v>63.34894712920155</v>
+        <v>57.83147724535762</v>
       </c>
       <c r="E3">
-        <v>0.4172891320107603</v>
+        <v>0.4175986545536549</v>
       </c>
       <c r="F3">
         <v>2588.449924639433</v>
@@ -9613,37 +9613,37 @@
         <v>3000</v>
       </c>
       <c r="C4">
-        <v>6074.883946474576</v>
+        <v>6030.051729519032</v>
       </c>
       <c r="D4">
-        <v>64.6486542019183</v>
+        <v>60.71717949474831</v>
       </c>
       <c r="E4">
-        <v>0.476475297502764</v>
+        <v>0.4768424550386773</v>
       </c>
       <c r="F4">
-        <v>2876.64577273829</v>
+        <v>2847.844530786419</v>
       </c>
       <c r="G4">
-        <v>-123.3542272617096</v>
+        <v>-152.155469213581</v>
       </c>
       <c r="H4">
-        <v>123.3542272617096</v>
+        <v>152.155469213581</v>
       </c>
       <c r="I4">
-        <v>180744.7895957442</v>
+        <v>184712.3003098799</v>
       </c>
       <c r="J4">
-        <v>355.9020759505715</v>
+        <v>370.3026969265072</v>
       </c>
       <c r="K4">
-        <v>4.111807575390322</v>
+        <v>5.071848973786033</v>
       </c>
       <c r="L4">
-        <v>16.767151903681</v>
+        <v>17.24717260287886</v>
       </c>
       <c r="M4">
-        <v>1.306808048633909</v>
+        <v>1.178210310232881</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -9654,37 +9654,37 @@
         <v>3000</v>
       </c>
       <c r="C5">
-        <v>6156.794307311377</v>
+        <v>6126.228713206215</v>
       </c>
       <c r="D5">
-        <v>66.37482486540661</v>
+        <v>64.26315991399174</v>
       </c>
       <c r="E5">
-        <v>0.4650870453292085</v>
+        <v>0.4653301572448232</v>
       </c>
       <c r="F5">
-        <v>2840.286869107766</v>
+        <v>2817.727680627593</v>
       </c>
       <c r="G5">
-        <v>-159.7131308922344</v>
+        <v>-182.2723193724073</v>
       </c>
       <c r="H5">
-        <v>159.7131308922344</v>
+        <v>182.2723193724073</v>
       </c>
       <c r="I5">
-        <v>128999.2877902961</v>
+        <v>134215.9330097189</v>
       </c>
       <c r="J5">
-        <v>290.5057609311258</v>
+        <v>307.6259044084739</v>
       </c>
       <c r="K5">
-        <v>5.323771029741147</v>
+        <v>6.075743979080244</v>
       </c>
       <c r="L5">
-        <v>12.95269161236771</v>
+        <v>13.52336306161265</v>
       </c>
       <c r="M5">
-        <v>1.05121001906014</v>
+        <v>0.825750147868392</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -9695,37 +9695,37 @@
         <v>3000</v>
       </c>
       <c r="C6">
-        <v>6288.705560111588</v>
+        <v>6311.398396717946</v>
       </c>
       <c r="D6">
-        <v>72.928467658887</v>
+        <v>76.35381227376567</v>
       </c>
       <c r="E6">
-        <v>0.4060848025505603</v>
+        <v>0.4059132792265963</v>
       </c>
       <c r="F6">
-        <v>2478.06755049886</v>
+        <v>2465.055457530236</v>
       </c>
       <c r="G6">
-        <v>-521.9324495011401</v>
+        <v>-534.9445424697637</v>
       </c>
       <c r="H6">
-        <v>521.9324495011401</v>
+        <v>534.9445424697637</v>
       </c>
       <c r="I6">
-        <v>164852.8363032871</v>
+        <v>172203.3656368354</v>
       </c>
       <c r="J6">
-        <v>348.3624330736294</v>
+        <v>364.4555639237964</v>
       </c>
       <c r="K6">
-        <v>17.39774831670467</v>
+        <v>17.83148474899212</v>
       </c>
       <c r="L6">
-        <v>14.06395578845195</v>
+        <v>14.60039348345752</v>
       </c>
       <c r="M6">
-        <v>-0.6216223750219388</v>
+        <v>-0.7708001584386742</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -9736,37 +9736,37 @@
         <v>4000</v>
       </c>
       <c r="C7">
-        <v>6365.449977879326</v>
+        <v>6392.270282877734</v>
       </c>
       <c r="D7">
-        <v>73.31006266977211</v>
+        <v>76.80561966236792</v>
       </c>
       <c r="E7">
-        <v>0.6220231830861283</v>
+        <v>0.6217595259902424</v>
       </c>
       <c r="F7">
-        <v>3952.581821071373</v>
+        <v>3968.809451872494</v>
       </c>
       <c r="G7">
-        <v>-47.41817892862719</v>
+        <v>-31.19054812750619</v>
       </c>
       <c r="H7">
-        <v>47.41817892862719</v>
+        <v>31.19054812750619</v>
       </c>
       <c r="I7">
-        <v>132331.9657812112</v>
+        <v>137957.2625679672</v>
       </c>
       <c r="J7">
-        <v>288.173582244629</v>
+        <v>297.8025607645383</v>
       </c>
       <c r="K7">
-        <v>1.18545447321568</v>
+        <v>0.7797637031876548</v>
       </c>
       <c r="L7">
-        <v>11.4882555254047</v>
+        <v>11.83626752740355</v>
       </c>
       <c r="M7">
-        <v>-0.9160036804490874</v>
+        <v>-1.048053293237465</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -9777,37 +9777,37 @@
         <v>6000</v>
       </c>
       <c r="C8">
-        <v>6476.36832655664</v>
+        <v>6534.042389774485</v>
       </c>
       <c r="D8">
-        <v>77.07089127052626</v>
+        <v>83.30226838580624</v>
       </c>
       <c r="E8">
-        <v>0.8435909406539719</v>
+        <v>0.84277319487376</v>
       </c>
       <c r="F8">
-        <v>5372.404267393573</v>
+        <v>5397.699365410037</v>
       </c>
       <c r="G8">
-        <v>-627.5957326064272</v>
+        <v>-602.300634589963</v>
       </c>
       <c r="H8">
-        <v>627.5957326064272</v>
+        <v>602.300634589963</v>
       </c>
       <c r="I8">
-        <v>175922.705415309</v>
+        <v>175425.3945445514</v>
       </c>
       <c r="J8">
-        <v>344.743940638262</v>
+        <v>348.5522397354425</v>
       </c>
       <c r="K8">
-        <v>10.45992887677379</v>
+        <v>10.03834390983272</v>
       </c>
       <c r="L8">
-        <v>11.31686775063288</v>
+        <v>11.53661359114174</v>
       </c>
       <c r="M8">
-        <v>-2.586162335152449</v>
+        <v>-2.62346209517358</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -9818,37 +9818,37 @@
         <v>7000</v>
       </c>
       <c r="C9">
-        <v>6636.140366213672</v>
+        <v>6760.455235626022</v>
       </c>
       <c r="D9">
-        <v>85.34100610917685</v>
+        <v>97.61332613237931</v>
       </c>
       <c r="E9">
-        <v>0.873077155742622</v>
+        <v>0.8711374778628178</v>
       </c>
       <c r="F9">
-        <v>5589.312931044017</v>
+        <v>5643.816756004559</v>
       </c>
       <c r="G9">
-        <v>-1410.687068955983</v>
+        <v>-1356.183243995441</v>
       </c>
       <c r="H9">
-        <v>1410.687068955983</v>
+        <v>1356.183243995441</v>
       </c>
       <c r="I9">
-        <v>435082.0341444965</v>
+        <v>413112.1940801867</v>
       </c>
       <c r="J9">
-        <v>497.0215303979364</v>
+        <v>492.4995260582995</v>
       </c>
       <c r="K9">
-        <v>20.1526724136569</v>
+        <v>19.37404634279202</v>
       </c>
       <c r="L9">
-        <v>12.57912555963631</v>
+        <v>12.6562468413775</v>
       </c>
       <c r="M9">
-        <v>-4.632094834329227</v>
+        <v>-4.610353336381583</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -9859,37 +9859,37 @@
         <v>6000</v>
       </c>
       <c r="C10">
-        <v>6646.01541280249</v>
+        <v>6709.936987572555</v>
       </c>
       <c r="D10">
-        <v>77.79441015714096</v>
+        <v>82.8001687137947</v>
       </c>
       <c r="E10">
-        <v>1.126318026086184</v>
+        <v>1.125457985532318</v>
       </c>
       <c r="F10">
-        <v>7737.458434018778</v>
+        <v>7894.691288256654</v>
       </c>
       <c r="G10">
-        <v>1737.458434018778</v>
+        <v>1894.691288256654</v>
       </c>
       <c r="H10">
-        <v>1737.458434018778</v>
+        <v>1894.691288256654</v>
       </c>
       <c r="I10">
-        <v>758042.0061193078</v>
+        <v>810205.0545446207</v>
       </c>
       <c r="J10">
-        <v>652.0761433505417</v>
+        <v>667.7734963330938</v>
       </c>
       <c r="K10">
-        <v>28.95764056697964</v>
+        <v>31.5781881376109</v>
       </c>
       <c r="L10">
-        <v>14.62643993555423</v>
+        <v>15.02148950340667</v>
       </c>
       <c r="M10">
-        <v>-0.8661449053876666</v>
+        <v>-0.5629237262885751</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -9900,37 +9900,37 @@
         <v>10000</v>
       </c>
       <c r="C11">
-        <v>6676.136356341646</v>
+        <v>6700.721456374573</v>
       </c>
       <c r="D11">
-        <v>73.02706349534252</v>
+        <v>73.598598722617</v>
       </c>
       <c r="E11">
-        <v>1.709487223255612</v>
+        <v>1.708937650472951</v>
       </c>
       <c r="F11">
-        <v>11652.36234137816</v>
+        <v>11771.8134091947</v>
       </c>
       <c r="G11">
-        <v>1652.362341378155</v>
+        <v>1771.813409194696</v>
       </c>
       <c r="H11">
-        <v>1652.362341378155</v>
+        <v>1771.813409194696</v>
       </c>
       <c r="I11">
-        <v>977181.9284621291</v>
+        <v>1068995.910373233</v>
       </c>
       <c r="J11">
-        <v>763.2190542424987</v>
+        <v>790.4445977621607</v>
       </c>
       <c r="K11">
-        <v>16.52362341378155</v>
+        <v>17.71813409194696</v>
       </c>
       <c r="L11">
-        <v>14.83723809980171</v>
+        <v>15.32111667991115</v>
       </c>
       <c r="M11">
-        <v>1.424977410934359</v>
+        <v>1.765978119496415</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -9941,37 +9941,37 @@
         <v>12000</v>
       </c>
       <c r="C12">
-        <v>6749.148202562081</v>
+        <v>6772.028566828938</v>
       </c>
       <c r="D12">
-        <v>73.02554176785172</v>
+        <v>73.36944989579182</v>
       </c>
       <c r="E12">
-        <v>1.778070702137963</v>
+        <v>1.777469976130866</v>
       </c>
       <c r="F12">
-        <v>12000.54115013184</v>
+        <v>12045.2716178742</v>
       </c>
       <c r="G12">
-        <v>0.5411501318449154</v>
+        <v>45.27161787420118</v>
       </c>
       <c r="H12">
-        <v>0.5411501318449154</v>
+        <v>45.27161787420118</v>
       </c>
       <c r="I12">
-        <v>879463.7649002627</v>
+        <v>962301.2712744044</v>
       </c>
       <c r="J12">
-        <v>686.9512638314334</v>
+        <v>715.9272997733648</v>
       </c>
       <c r="K12">
-        <v>0.004509584432040963</v>
+        <v>0.3772634822850099</v>
       </c>
       <c r="L12">
-        <v>13.35396524826474</v>
+        <v>13.82673136014853</v>
       </c>
       <c r="M12">
-        <v>1.583971264501662</v>
+        <v>2.013024901624151</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -9982,37 +9982,37 @@
         <v>14000</v>
       </c>
       <c r="C13">
-        <v>6810.681230180669</v>
+        <v>6822.621306740525</v>
       </c>
       <c r="D13">
-        <v>71.87629035292542</v>
+        <v>71.09177889737136</v>
       </c>
       <c r="E13">
-        <v>2.116873447634368</v>
+        <v>2.11651370382668</v>
       </c>
       <c r="F13">
-        <v>14488.12895493712</v>
+        <v>14537.44992885985</v>
       </c>
       <c r="G13">
-        <v>488.1289549371177</v>
+        <v>537.4499288598454</v>
       </c>
       <c r="H13">
-        <v>488.1289549371177</v>
+        <v>537.4499288598454</v>
       </c>
       <c r="I13">
-        <v>821173.4114227846</v>
+        <v>901078.6489795907</v>
       </c>
       <c r="J13">
-        <v>668.8765084774046</v>
+        <v>699.7020842357721</v>
       </c>
       <c r="K13">
-        <v>3.486635392407984</v>
+        <v>3.83892806328461</v>
       </c>
       <c r="L13">
-        <v>12.45693526136867</v>
+        <v>12.91874924225181</v>
       </c>
       <c r="M13">
-        <v>2.356548625914936</v>
+        <v>2.827816946146822</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -10023,37 +10023,37 @@
         <v>8000</v>
       </c>
       <c r="C14">
-        <v>6903.819859595233</v>
+        <v>6930.981295089457</v>
       </c>
       <c r="D14">
-        <v>74.0025242590892</v>
+        <v>74.81859984252746</v>
       </c>
       <c r="E14">
-        <v>1.101125937133618</v>
+        <v>1.100671829786836</v>
       </c>
       <c r="F14">
-        <v>7534.473816021619</v>
+        <v>7546.68603697735</v>
       </c>
       <c r="G14">
-        <v>-465.5261839783807</v>
+        <v>-453.3139630226497</v>
       </c>
       <c r="H14">
-        <v>465.5261839783807</v>
+        <v>453.3139630226497</v>
       </c>
       <c r="I14">
-        <v>770801.8461350086</v>
+        <v>843113.2239872332</v>
       </c>
       <c r="J14">
-        <v>651.930648102486</v>
+        <v>679.1697408013453</v>
       </c>
       <c r="K14">
-        <v>5.819077299729758</v>
+        <v>5.66642453778312</v>
       </c>
       <c r="L14">
-        <v>11.9037804312321</v>
+        <v>12.31438885021276</v>
       </c>
       <c r="M14">
-        <v>1.703730045847176</v>
+        <v>2.245853070888897</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -10064,37 +10064,37 @@
         <v>3000</v>
       </c>
       <c r="C15">
-        <v>6988.394256849315</v>
+        <v>7021.831711628186</v>
       </c>
       <c r="D15">
-        <v>75.0597115585885</v>
+        <v>76.42178151214756</v>
       </c>
       <c r="E15">
-        <v>0.4184885352403107</v>
+        <v>0.4185626839907288</v>
       </c>
       <c r="F15">
-        <v>2911.769445883824</v>
+        <v>2925.612610195734</v>
       </c>
       <c r="G15">
-        <v>-88.23055411617588</v>
+        <v>-74.38738980426615</v>
       </c>
       <c r="H15">
-        <v>88.23055411617588</v>
+        <v>74.38738980426615</v>
       </c>
       <c r="I15">
-        <v>712108.2141769039</v>
+        <v>778684.0132006685</v>
       </c>
       <c r="J15">
-        <v>608.5691024112314</v>
+        <v>632.6480214938776</v>
       </c>
       <c r="K15">
-        <v>2.941018470539196</v>
+        <v>2.479579660142205</v>
       </c>
       <c r="L15">
-        <v>11.21433720348649</v>
+        <v>11.55786506636118</v>
       </c>
       <c r="M15">
-        <v>1.680143265265091</v>
+        <v>2.293420684068784</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -10105,37 +10105,37 @@
         <v>4000</v>
       </c>
       <c r="C16">
-        <v>7130.030207756607</v>
+        <v>7214.377012388379</v>
       </c>
       <c r="D16">
-        <v>81.71733549345883</v>
+        <v>88.03413343695209</v>
       </c>
       <c r="E16">
-        <v>0.4849285118369725</v>
+        <v>0.4846030524246569</v>
       </c>
       <c r="F16">
-        <v>3365.561330994235</v>
+        <v>3384.748622155903</v>
       </c>
       <c r="G16">
-        <v>-634.4386690057654</v>
+        <v>-615.2513778440966</v>
       </c>
       <c r="H16">
-        <v>634.4386690057654</v>
+        <v>615.2513778440966</v>
       </c>
       <c r="I16">
-        <v>689994.229216397</v>
+        <v>750101.8878248392</v>
       </c>
       <c r="J16">
-        <v>610.4169285965553</v>
+        <v>631.4054040903219</v>
       </c>
       <c r="K16">
-        <v>15.86096672514413</v>
+        <v>15.38128444610242</v>
       </c>
       <c r="L16">
-        <v>11.54623931217632</v>
+        <v>11.83096645062841</v>
       </c>
       <c r="M16">
-        <v>0.6357042075341227</v>
+        <v>1.323518416173727</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -10146,37 +10146,37 @@
         <v>3000</v>
       </c>
       <c r="C17">
-        <v>7173.680437306519</v>
+        <v>7225.427329388639</v>
       </c>
       <c r="D17">
-        <v>77.91062489910416</v>
+        <v>80.33575179328291</v>
       </c>
       <c r="E17">
-        <v>0.4603978785665874</v>
+        <v>0.4603171771284471</v>
       </c>
       <c r="F17">
-        <v>3354.090356550351</v>
+        <v>3398.032126753251</v>
       </c>
       <c r="G17">
-        <v>354.0903565503513</v>
+        <v>398.0321267532509</v>
       </c>
       <c r="H17">
-        <v>354.0903565503513</v>
+        <v>398.0321267532509</v>
       </c>
       <c r="I17">
-        <v>652353.2793087676</v>
+        <v>710657.0668983643</v>
       </c>
       <c r="J17">
-        <v>593.3284904601417</v>
+        <v>615.8471856011838</v>
       </c>
       <c r="K17">
-        <v>11.80301188501171</v>
+        <v>13.2677375584417</v>
       </c>
       <c r="L17">
-        <v>11.56335748369868</v>
+        <v>11.92675119114929</v>
       </c>
       <c r="M17">
-        <v>1.250799478436798</v>
+        <v>2.00327099966215</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -10187,37 +10187,37 @@
         <v>5000</v>
       </c>
       <c r="C18">
-        <v>7504.646466202295</v>
+        <v>7756.855585203256</v>
       </c>
       <c r="D18">
-        <v>103.2161652987714</v>
+        <v>125.4450021954163</v>
       </c>
       <c r="E18">
-        <v>0.4321017126122614</v>
+        <v>0.4297810603472692</v>
       </c>
       <c r="F18">
-        <v>2944.760924673178</v>
+        <v>2965.506249535156</v>
       </c>
       <c r="G18">
-        <v>-2055.239075326822</v>
+        <v>-2034.493750464844</v>
       </c>
       <c r="H18">
-        <v>2055.239075326822</v>
+        <v>2034.493750464844</v>
       </c>
       <c r="I18">
-        <v>875581.6778988601</v>
+        <v>924938.8015097483</v>
       </c>
       <c r="J18">
-        <v>684.6979020143092</v>
+        <v>704.5125959051625</v>
       </c>
       <c r="K18">
-        <v>41.10478150653643</v>
+        <v>40.68987500929688</v>
       </c>
       <c r="L18">
-        <v>13.40969648512604</v>
+        <v>13.72444642978352</v>
       </c>
       <c r="M18">
-        <v>-1.917786085008542</v>
+        <v>-1.136650995285024</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -10228,37 +10228,37 @@
         <v>5000</v>
       </c>
       <c r="C19">
-        <v>7629.383780290358</v>
+        <v>7896.646016303473</v>
       </c>
       <c r="D19">
-        <v>105.3682801777006</v>
+        <v>126.8795450858963</v>
       </c>
       <c r="E19">
-        <v>0.6253569571276857</v>
+        <v>0.6229015946077824</v>
       </c>
       <c r="F19">
-        <v>4732.266930528302</v>
+        <v>4900.895476933608</v>
       </c>
       <c r="G19">
-        <v>-267.7330694716984</v>
+        <v>-99.10452306639218</v>
       </c>
       <c r="H19">
-        <v>267.7330694716984</v>
+        <v>99.10452306639218</v>
       </c>
       <c r="I19">
-        <v>828293.402521794</v>
+        <v>871108.3841557759</v>
       </c>
       <c r="J19">
-        <v>660.1705589235673</v>
+        <v>668.9003563264113</v>
       </c>
       <c r="K19">
-        <v>5.354661389433968</v>
+        <v>1.982090461327844</v>
       </c>
       <c r="L19">
-        <v>12.9358708912618</v>
+        <v>13.03371960810965</v>
       </c>
       <c r="M19">
-        <v>-2.394589030093824</v>
+        <v>-1.345326636294541</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -10269,37 +10269,37 @@
         <v>8000</v>
       </c>
       <c r="C20">
-        <v>7822.17791833947</v>
+        <v>8155.730638912728</v>
       </c>
       <c r="D20">
-        <v>114.1108659648417</v>
+        <v>140.1000528382322</v>
       </c>
       <c r="E20">
-        <v>0.8615051531218308</v>
+        <v>0.8565864126318186</v>
       </c>
       <c r="F20">
-        <v>6524.966766415497</v>
+        <v>6762.012271523397</v>
       </c>
       <c r="G20">
-        <v>-1475.033233584503</v>
+        <v>-1237.987728476603</v>
       </c>
       <c r="H20">
-        <v>1475.033233584503</v>
+        <v>1237.987728476603</v>
       </c>
       <c r="I20">
-        <v>903150.6046138474</v>
+        <v>907858.6748059361</v>
       </c>
       <c r="J20">
-        <v>705.4407075158416</v>
+        <v>700.5163214458663</v>
       </c>
       <c r="K20">
-        <v>18.43791541980629</v>
+        <v>15.47484660595753</v>
       </c>
       <c r="L20">
-        <v>13.24154003173649</v>
+        <v>13.16933777465676</v>
       </c>
       <c r="M20">
-        <v>-4.331860040703934</v>
+        <v>-3.051859220720015</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -10310,37 +10310,37 @@
         <v>3000</v>
       </c>
       <c r="C21">
-        <v>7711.280466705475</v>
+        <v>7859.145527847467</v>
       </c>
       <c r="D21">
-        <v>91.61003420495804</v>
+        <v>96.43153644788291</v>
       </c>
       <c r="E21">
-        <v>0.8246734848721274</v>
+        <v>0.8221958187516984</v>
       </c>
       <c r="F21">
-        <v>6928.99243895248</v>
+        <v>7226.809025588886</v>
       </c>
       <c r="G21">
-        <v>3928.99243895248</v>
+        <v>4226.809025588886</v>
       </c>
       <c r="H21">
-        <v>3928.99243895248</v>
+        <v>4226.809025588886</v>
       </c>
       <c r="I21">
-        <v>1668089.077283948</v>
+        <v>1800387.930805606</v>
       </c>
       <c r="J21">
-        <v>875.1013249598752</v>
+        <v>886.1106742954989</v>
       </c>
       <c r="K21">
-        <v>130.9664146317493</v>
+        <v>140.8936341862962</v>
       </c>
       <c r="L21">
-        <v>19.43758606331612</v>
+        <v>19.89166916474305</v>
       </c>
       <c r="M21">
-        <v>0.9977382070798814</v>
+        <v>2.357416394267291</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -10351,37 +10351,37 @@
         <v>8000</v>
       </c>
       <c r="C22">
-        <v>7767.885457552824</v>
+        <v>7879.31469165155</v>
       </c>
       <c r="D22">
-        <v>88.10952986919712</v>
+        <v>88.80529918350291</v>
       </c>
       <c r="E22">
-        <v>1.116674353821603</v>
+        <v>1.114443859631739</v>
       </c>
       <c r="F22">
-        <v>8788.536226752074</v>
+        <v>8953.66773652896</v>
       </c>
       <c r="G22">
-        <v>788.5362267520741</v>
+        <v>953.6677365289597</v>
       </c>
       <c r="H22">
-        <v>788.5362267520741</v>
+        <v>953.6677365289597</v>
       </c>
       <c r="I22">
-        <v>1615774.092464771</v>
+        <v>1755842.641850139</v>
       </c>
       <c r="J22">
-        <v>870.7730700494852</v>
+        <v>889.4885274071719</v>
       </c>
       <c r="K22">
-        <v>9.856702834400926</v>
+        <v>11.920846706612</v>
       </c>
       <c r="L22">
-        <v>18.95854190187036</v>
+        <v>19.4931280418365</v>
       </c>
       <c r="M22">
-        <v>1.908256365388445</v>
+        <v>3.420616987739555</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -10392,37 +10392,37 @@
         <v>12000</v>
       </c>
       <c r="C23">
-        <v>7814.177679942083</v>
+        <v>7882.96075580743</v>
       </c>
       <c r="D23">
-        <v>83.92779912120332</v>
+        <v>80.28937568074068</v>
       </c>
       <c r="E23">
-        <v>1.692105523481923</v>
+        <v>1.690270953043106</v>
       </c>
       <c r="F23">
-        <v>13429.72305695808</v>
+        <v>13617.02025582421</v>
       </c>
       <c r="G23">
-        <v>1429.723056958079</v>
+        <v>1617.020255824211</v>
       </c>
       <c r="H23">
-        <v>1429.723056958079</v>
+        <v>1617.020255824211</v>
       </c>
       <c r="I23">
-        <v>1636170.94613776</v>
+        <v>1796743.20689279</v>
       </c>
       <c r="J23">
-        <v>897.3897360927516</v>
+        <v>924.1328954270308</v>
       </c>
       <c r="K23">
-        <v>11.91435880798399</v>
+        <v>13.47516879853509</v>
       </c>
       <c r="L23">
-        <v>18.6231046116853</v>
+        <v>19.20655855406024</v>
       </c>
       <c r="M23">
-        <v>3.444859224876772</v>
+        <v>5.042153402535757</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -10433,37 +10433,37 @@
         <v>12000</v>
       </c>
       <c r="C24">
-        <v>7840.644604412442</v>
+        <v>7854.162819462396</v>
       </c>
       <c r="D24">
-        <v>78.18171165611891</v>
+        <v>69.38064447816321</v>
       </c>
       <c r="E24">
-        <v>1.753312272762279</v>
+        <v>1.752508199245115</v>
       </c>
       <c r="F24">
-        <v>14043.38995471775</v>
+        <v>14154.43802114039</v>
       </c>
       <c r="G24">
-        <v>2043.38995471775</v>
+        <v>2154.438021140391</v>
       </c>
       <c r="H24">
-        <v>2043.38995471775</v>
+        <v>2154.438021140391</v>
       </c>
       <c r="I24">
-        <v>1751592.38072429</v>
+        <v>1926055.024167451</v>
       </c>
       <c r="J24">
-        <v>949.4806551211606</v>
+        <v>980.055855686729</v>
       </c>
       <c r="K24">
-        <v>17.02824962264792</v>
+        <v>17.95365017616993</v>
       </c>
       <c r="L24">
-        <v>18.55061120309269</v>
+        <v>19.14960817324704</v>
       </c>
       <c r="M24">
-        <v>5.407978812113201</v>
+        <v>6.952723974531408</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -10474,37 +10474,37 @@
         <v>16000</v>
       </c>
       <c r="C25">
-        <v>7900.800836893916</v>
+        <v>7890.78867994774</v>
       </c>
       <c r="D25">
-        <v>76.37916373865443</v>
+        <v>66.10516607888127</v>
       </c>
       <c r="E25">
-        <v>2.107697219532494</v>
+        <v>2.107630404532515</v>
       </c>
       <c r="F25">
-        <v>16763.15316491382</v>
+        <v>16770.28832429651</v>
       </c>
       <c r="G25">
-        <v>763.1531649138196</v>
+        <v>770.2883242965145</v>
       </c>
       <c r="H25">
-        <v>763.1531649138196</v>
+        <v>770.2883242965145</v>
       </c>
       <c r="I25">
-        <v>1700758.049089233</v>
+        <v>1868111.071053541</v>
       </c>
       <c r="J25">
-        <v>941.3794598947545</v>
+        <v>970.9355282349806</v>
       </c>
       <c r="K25">
-        <v>4.769707280711373</v>
+        <v>4.814302026853215</v>
       </c>
       <c r="L25">
-        <v>17.95144146733698</v>
+        <v>18.52633399296905</v>
       </c>
       <c r="M25">
-        <v>6.26519345448625</v>
+        <v>7.8113797960373</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -10515,37 +10515,37 @@
         <v>10000</v>
       </c>
       <c r="C26">
-        <v>8032.401667614898</v>
+        <v>8058.455814972745</v>
       </c>
       <c r="D26">
-        <v>81.90133043688712</v>
+        <v>76.26136297349368</v>
       </c>
       <c r="E26">
-        <v>1.11550910961579</v>
+        <v>1.114697900275149</v>
       </c>
       <c r="F26">
-        <v>8783.879803880096</v>
+        <v>8757.92890892574</v>
       </c>
       <c r="G26">
-        <v>-1216.120196119904</v>
+        <v>-1242.07109107426</v>
       </c>
       <c r="H26">
-        <v>1216.120196119904</v>
+        <v>1242.07109107426</v>
       </c>
       <c r="I26">
-        <v>1691515.977519294</v>
+        <v>1854553.96789641</v>
       </c>
       <c r="J26">
-        <v>952.8269905708024</v>
+        <v>982.232843353284</v>
       </c>
       <c r="K26">
-        <v>12.16120196119904</v>
+        <v>12.4207109107426</v>
       </c>
       <c r="L26">
-        <v>17.71018148791456</v>
+        <v>18.27193303120961</v>
       </c>
       <c r="M26">
-        <v>4.91359321317695</v>
+        <v>6.456997564633578</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -10556,37 +10556,37 @@
         <v>2000</v>
       </c>
       <c r="C27">
-        <v>7947.543020344239</v>
+        <v>7832.635745865207</v>
       </c>
       <c r="D27">
-        <v>65.22533266613259</v>
+        <v>46.05321976539051</v>
       </c>
       <c r="E27">
-        <v>0.4018046917688251</v>
+        <v>0.4022406043997565</v>
       </c>
       <c r="F27">
-        <v>3395.742776150753</v>
+        <v>3404.889055506665</v>
       </c>
       <c r="G27">
-        <v>1395.742776150753</v>
+        <v>1404.889055506665</v>
       </c>
       <c r="H27">
-        <v>1395.742776150753</v>
+        <v>1404.889055506665</v>
       </c>
       <c r="I27">
-        <v>1701779.254305603</v>
+        <v>1859320.33951185</v>
       </c>
       <c r="J27">
-        <v>970.5436219940004</v>
+        <v>999.1390918394193</v>
       </c>
       <c r="K27">
-        <v>69.78713880753766</v>
+        <v>70.24445277533323</v>
       </c>
       <c r="L27">
-        <v>19.79325978069948</v>
+        <v>20.35083382097456</v>
       </c>
       <c r="M27">
-        <v>6.262002935905992</v>
+        <v>7.753839476623193</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -10597,37 +10597,37 @@
         <v>5000</v>
       </c>
       <c r="C28">
-        <v>8127.669842578275</v>
+        <v>8098.202017604459</v>
       </c>
       <c r="D28">
-        <v>76.71548162292292</v>
+        <v>68.00452496277661</v>
       </c>
       <c r="E28">
-        <v>0.4979539075412898</v>
+        <v>0.4978848473314668</v>
       </c>
       <c r="F28">
-        <v>3885.619833119709</v>
+        <v>3818.03672184905</v>
       </c>
       <c r="G28">
-        <v>-1114.380166880291</v>
+        <v>-1181.96327815095</v>
       </c>
       <c r="H28">
-        <v>1114.380166880291</v>
+        <v>1181.96327815095</v>
       </c>
       <c r="I28">
-        <v>1684089.404383701</v>
+        <v>1841540.218411292</v>
       </c>
       <c r="J28">
-        <v>976.0757967973193</v>
+        <v>1006.17079131294</v>
       </c>
       <c r="K28">
-        <v>22.28760333760582</v>
+        <v>23.639265563019</v>
       </c>
       <c r="L28">
-        <v>19.88919607134973</v>
+        <v>20.47731196489934</v>
       </c>
       <c r="M28">
-        <v>5.0848170395742</v>
+        <v>6.524936831275072</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -10638,37 +10638,37 @@
         <v>5000</v>
       </c>
       <c r="C29">
-        <v>8337.174641736907</v>
+        <v>8408.834762047776</v>
       </c>
       <c r="D29">
-        <v>89.99441337649378</v>
+        <v>92.26734691083068</v>
       </c>
       <c r="E29">
-        <v>0.4743304460324308</v>
+        <v>0.4737467301087414</v>
       </c>
       <c r="F29">
-        <v>3777.281598205075</v>
+        <v>3759.045143522405</v>
       </c>
       <c r="G29">
-        <v>-1222.718401794925</v>
+        <v>-1240.954856477595</v>
       </c>
       <c r="H29">
-        <v>1222.718401794925</v>
+        <v>1240.954856477595</v>
       </c>
       <c r="I29">
-        <v>1677087.585335709</v>
+        <v>1830370.91238922</v>
       </c>
       <c r="J29">
-        <v>985.2107080935269</v>
+        <v>1014.866497430149</v>
       </c>
       <c r="K29">
-        <v>24.4543680358985</v>
+        <v>24.81909712955189</v>
       </c>
       <c r="L29">
-        <v>20.05827651448116</v>
+        <v>20.63811882284944</v>
       </c>
       <c r="M29">
-        <v>3.796597429309471</v>
+        <v>5.246252597553942</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -10679,37 +10679,37 @@
         <v>3000</v>
       </c>
       <c r="C30">
-        <v>8352.951091788282</v>
+        <v>8364.229765123247</v>
       </c>
       <c r="D30">
-        <v>82.57261704398191</v>
+        <v>78.58011252729474</v>
       </c>
       <c r="E30">
-        <v>0.4248069916755233</v>
+        <v>0.4226699747584565</v>
       </c>
       <c r="F30">
-        <v>3641.394181187552</v>
+        <v>3653.612678508636</v>
       </c>
       <c r="G30">
-        <v>641.3941811875525</v>
+        <v>653.6126785086362</v>
       </c>
       <c r="H30">
-        <v>641.3941811875525</v>
+        <v>653.6126785086362</v>
       </c>
       <c r="I30">
-        <v>1631883.974990193</v>
+        <v>1780258.006000577</v>
       </c>
       <c r="J30">
-        <v>972.9315464183136</v>
+        <v>1001.964575325809</v>
       </c>
       <c r="K30">
-        <v>21.37980603958508</v>
+        <v>21.78708928362121</v>
       </c>
       <c r="L30">
-        <v>20.10547399752059</v>
+        <v>20.67915348216271</v>
       </c>
       <c r="M30">
-        <v>4.50375223107384</v>
+        <v>5.966137749808373</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -10720,37 +10720,37 @@
         <v>4000</v>
       </c>
       <c r="C31">
-        <v>8333.564865662838</v>
+        <v>8260.897393882306</v>
       </c>
       <c r="D31">
-        <v>72.37673272703937</v>
+        <v>60.38886415047108</v>
       </c>
       <c r="E31">
-        <v>0.6108199278257516</v>
+        <v>0.6090323246615289</v>
       </c>
       <c r="F31">
-        <v>5275.213438333793</v>
+        <v>5259.039735758859</v>
       </c>
       <c r="G31">
-        <v>1275.213438333793</v>
+        <v>1259.039735758859</v>
       </c>
       <c r="H31">
-        <v>1275.213438333793</v>
+        <v>1259.039735758859</v>
       </c>
       <c r="I31">
-        <v>1631686.917690776</v>
+        <v>1773531.214628824</v>
       </c>
       <c r="J31">
-        <v>983.3550599326405</v>
+        <v>1010.829236030397</v>
       </c>
       <c r="K31">
-        <v>31.88033595834484</v>
+        <v>31.47599339397147</v>
       </c>
       <c r="L31">
-        <v>20.51150372030763</v>
+        <v>21.05145830670785</v>
       </c>
       <c r="M31">
-        <v>5.752811259836198</v>
+        <v>7.159367927465902</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -10761,37 +10761,37 @@
         <v>6000</v>
       </c>
       <c r="C32">
-        <v>8333.872267210936</v>
+        <v>8202.779747206065</v>
       </c>
       <c r="D32">
-        <v>65.16979960914523</v>
+        <v>48.53821306779989</v>
       </c>
       <c r="E32">
-        <v>0.8473499817220641</v>
+        <v>0.8440737070746839</v>
       </c>
       <c r="F32">
-        <v>7241.762003854039</v>
+        <v>7127.900744250745</v>
       </c>
       <c r="G32">
-        <v>1241.762003854039</v>
+        <v>1127.900744250745</v>
       </c>
       <c r="H32">
-        <v>1241.762003854039</v>
+        <v>1127.900744250745</v>
       </c>
       <c r="I32">
-        <v>1628696.449574937</v>
+        <v>1756818.843770576</v>
       </c>
       <c r="J32">
-        <v>991.9686247300203</v>
+        <v>1014.731619637742</v>
       </c>
       <c r="K32">
-        <v>20.69603339756732</v>
+        <v>18.79834573751242</v>
       </c>
       <c r="L32">
-        <v>20.51765470954962</v>
+        <v>20.97635455440133</v>
       </c>
       <c r="M32">
-        <v>6.95467365908781</v>
+        <v>8.243361096619671</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -10802,37 +10802,37 @@
         <v>7000</v>
       </c>
       <c r="C33">
-        <v>8403.500359133148</v>
+        <v>8274.940165842814</v>
       </c>
       <c r="D33">
-        <v>65.61562884045189</v>
+        <v>50.90043362469485</v>
       </c>
       <c r="E33">
-        <v>0.8255047583977313</v>
+        <v>0.8245689935576525</v>
       </c>
       <c r="F33">
-        <v>6926.467290832113</v>
+        <v>6784.199126127964</v>
       </c>
       <c r="G33">
-        <v>-73.53270916788733</v>
+        <v>-215.8008738720364</v>
       </c>
       <c r="H33">
-        <v>73.53270916788733</v>
+        <v>215.8008738720364</v>
       </c>
       <c r="I33">
-        <v>1576332.275695667</v>
+        <v>1701649.526783265</v>
       </c>
       <c r="J33">
-        <v>962.3416597118871</v>
+        <v>988.9596600969129</v>
       </c>
       <c r="K33">
-        <v>1.050467273826962</v>
+        <v>3.082869626743377</v>
       </c>
       <c r="L33">
-        <v>19.88968092130051</v>
+        <v>20.39914536318656</v>
       </c>
       <c r="M33">
-        <v>7.092372326401155</v>
+        <v>8.23997035648657</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -10843,37 +10843,37 @@
         <v>10000</v>
       </c>
       <c r="C34">
-        <v>8493.418300229268</v>
+        <v>8384.092637493026</v>
       </c>
       <c r="D34">
-        <v>68.04586006601876</v>
+        <v>56.72563742724654</v>
       </c>
       <c r="E34">
-        <v>1.122745144045616</v>
+        <v>1.122272964937981</v>
       </c>
       <c r="F34">
-        <v>9457.244623310624</v>
+        <v>9278.681932349202</v>
       </c>
       <c r="G34">
-        <v>-542.7553766893761</v>
+        <v>-721.3180676507982</v>
       </c>
       <c r="H34">
-        <v>542.7553766893761</v>
+        <v>721.3180676507982</v>
       </c>
       <c r="I34">
-        <v>1536277.623296591</v>
+        <v>1664732.346406272</v>
       </c>
       <c r="J34">
-        <v>949.2295883674335</v>
+        <v>980.5958603329718</v>
       </c>
       <c r="K34">
-        <v>5.427553766893761</v>
+        <v>7.213180676507982</v>
       </c>
       <c r="L34">
-        <v>19.43773944772529</v>
+        <v>19.98708396672785</v>
       </c>
       <c r="M34">
-        <v>6.618556834073626</v>
+        <v>7.574659975401739</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -10884,37 +10884,37 @@
         <v>15000</v>
       </c>
       <c r="C35">
-        <v>8576.625720793476</v>
+        <v>8479.833146695766</v>
       </c>
       <c r="D35">
-        <v>69.56201611583764</v>
+        <v>60.62712460479591</v>
       </c>
       <c r="E35">
-        <v>1.697788926965725</v>
+        <v>1.69813413070183</v>
       </c>
       <c r="F35">
-        <v>14486.90079472818</v>
+        <v>14267.26995001316</v>
       </c>
       <c r="G35">
-        <v>-513.0992052718211</v>
+        <v>-732.7300499868415</v>
       </c>
       <c r="H35">
-        <v>513.0992052718211</v>
+        <v>732.7300499868415</v>
       </c>
       <c r="I35">
-        <v>1497701.658786105</v>
+        <v>1630555.406398619</v>
       </c>
       <c r="J35">
-        <v>936.0135161524149</v>
+        <v>973.084775170968</v>
       </c>
       <c r="K35">
-        <v>3.420661368478808</v>
+        <v>4.884866999912277</v>
       </c>
       <c r="L35">
-        <v>18.95237344532388</v>
+        <v>19.5294410283395</v>
       </c>
       <c r="M35">
-        <v>6.163832759208672</v>
+        <v>6.88013042249651</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -10925,37 +10925,37 @@
         <v>15000</v>
       </c>
       <c r="C36">
-        <v>8641.640142216482</v>
+        <v>8542.143345554336</v>
       </c>
       <c r="D36">
-        <v>69.10725664655446</v>
+        <v>60.79543203017327</v>
       </c>
       <c r="E36">
-        <v>1.751559206033624</v>
+        <v>1.752857335832767</v>
       </c>
       <c r="F36">
-        <v>15159.46707172981</v>
+        <v>14967.2266507814</v>
       </c>
       <c r="G36">
-        <v>159.4670717298104</v>
+        <v>-32.77334921860165</v>
       </c>
       <c r="H36">
-        <v>159.4670717298104</v>
+        <v>32.77334921860165</v>
       </c>
       <c r="I36">
-        <v>1454399.543732575</v>
+        <v>1582629.485399218</v>
       </c>
       <c r="J36">
-        <v>913.1739148458678</v>
+        <v>945.4285567606042</v>
       </c>
       <c r="K36">
-        <v>1.063113811532069</v>
+        <v>0.2184889947906777</v>
       </c>
       <c r="L36">
-        <v>18.42621875021236</v>
+        <v>18.96147185088219</v>
       </c>
       <c r="M36">
-        <v>6.492627252337671</v>
+        <v>7.046726871600419</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -10966,37 +10966,37 @@
         <v>18000</v>
       </c>
       <c r="C37">
-        <v>8702.216333079465</v>
+        <v>8597.310001205267</v>
       </c>
       <c r="D37">
-        <v>68.2541500681973</v>
+        <v>60.23255439224912</v>
       </c>
       <c r="E37">
-        <v>2.103771355638452</v>
+        <v>2.106235177935884</v>
       </c>
       <c r="F37">
-        <v>18359.61807263353</v>
+        <v>18131.8153359689</v>
       </c>
       <c r="G37">
-        <v>359.618072633526</v>
+        <v>131.8153359688986</v>
       </c>
       <c r="H37">
-        <v>359.618072633526</v>
+        <v>131.8153359688986</v>
       </c>
       <c r="I37">
-        <v>1416540.275573491</v>
+        <v>1537907.936753429</v>
       </c>
       <c r="J37">
-        <v>897.3580336398009</v>
+        <v>922.1824647379841</v>
       </c>
       <c r="K37">
-        <v>1.997878181297367</v>
+        <v>0.7323074220494366</v>
       </c>
       <c r="L37">
-        <v>17.9568375911005</v>
+        <v>18.44063858148697</v>
       </c>
       <c r="M37">
-        <v>7.007811467156146</v>
+        <v>7.367297050050284</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -11007,37 +11007,37 @@
         <v>8000</v>
       </c>
       <c r="C38">
-        <v>8690.527625478759</v>
+        <v>8524.2786410361</v>
       </c>
       <c r="D38">
-        <v>60.25986430130697</v>
+        <v>46.90616293610752</v>
       </c>
       <c r="E38">
-        <v>1.096012448347242</v>
+        <v>1.097077693735999</v>
       </c>
       <c r="F38">
-        <v>9783.539719567618</v>
+        <v>9650.544508267296</v>
       </c>
       <c r="G38">
-        <v>1783.539719567618</v>
+        <v>1650.544508267296</v>
       </c>
       <c r="H38">
-        <v>1783.539719567618</v>
+        <v>1650.544508267296</v>
       </c>
       <c r="I38">
-        <v>1465553.43267632</v>
+        <v>1570863.193337259</v>
       </c>
       <c r="J38">
-        <v>921.9741915822402</v>
+        <v>942.4147437249093</v>
       </c>
       <c r="K38">
-        <v>22.29424649459522</v>
+        <v>20.6318063533412</v>
       </c>
       <c r="L38">
-        <v>18.07732117175313</v>
+        <v>18.50150435292736</v>
       </c>
       <c r="M38">
-        <v>8.755186112097668</v>
+        <v>8.960531142543864</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -11048,37 +11048,37 @@
         <v>5000</v>
       </c>
       <c r="C39">
-        <v>8935.440949574428</v>
+        <v>8918.511574154993</v>
       </c>
       <c r="D39">
-        <v>78.72521028074317</v>
+        <v>81.63883995438599</v>
       </c>
       <c r="E39">
-        <v>0.4175811700802267</v>
+        <v>0.4180797105366963</v>
       </c>
       <c r="F39">
-        <v>3516.107470065569</v>
+        <v>3447.67855597179</v>
       </c>
       <c r="G39">
-        <v>-1483.892529934431</v>
+        <v>-1552.32144402821</v>
       </c>
       <c r="H39">
-        <v>1483.892529934431</v>
+        <v>1552.32144402821</v>
       </c>
       <c r="I39">
-        <v>1485455.692344398</v>
+        <v>1593534.508803545</v>
       </c>
       <c r="J39">
-        <v>937.1611736998672</v>
+        <v>958.8987085979714</v>
       </c>
       <c r="K39">
-        <v>29.67785059868862</v>
+        <v>31.04642888056421</v>
       </c>
       <c r="L39">
-        <v>18.39084899410274</v>
+        <v>18.84055636718782</v>
       </c>
       <c r="M39">
-        <v>7.029914696432763</v>
+        <v>7.187636352528419</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -11089,37 +11089,37 @@
         <v>4000</v>
       </c>
       <c r="C40">
-        <v>8965.101451744025</v>
+        <v>8913.195636168135</v>
       </c>
       <c r="D40">
-        <v>73.81873946962862</v>
+        <v>72.94336216026164</v>
       </c>
       <c r="E40">
-        <v>0.4927759706055095</v>
+        <v>0.4929736452618883</v>
       </c>
       <c r="F40">
-        <v>4488.639262526345</v>
+        <v>4481.038514889085</v>
       </c>
       <c r="G40">
-        <v>488.6392625263452</v>
+        <v>481.0385148890855</v>
       </c>
       <c r="H40">
-        <v>488.6392625263452</v>
+        <v>481.0385148890855</v>
       </c>
       <c r="I40">
-        <v>1452648.130148027</v>
+        <v>1557688.812593102</v>
       </c>
       <c r="J40">
-        <v>925.3579655110902</v>
+        <v>946.3234403424744</v>
       </c>
       <c r="K40">
-        <v>12.21598156315863</v>
+        <v>12.02596287222714</v>
       </c>
       <c r="L40">
-        <v>18.2283524827621</v>
+        <v>18.66122495942569</v>
       </c>
       <c r="M40">
-        <v>7.647637599938513</v>
+        <v>7.791473207650906</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -11130,37 +11130,37 @@
         <v>4000</v>
       </c>
       <c r="C41">
-        <v>9008.6211614598</v>
+        <v>8937.28619251979</v>
       </c>
       <c r="D41">
-        <v>70.7888364942432</v>
+        <v>68.05808157940101</v>
       </c>
       <c r="E41">
-        <v>0.4712993129793436</v>
+        <v>0.4711283725367514</v>
       </c>
       <c r="F41">
-        <v>4287.435045949917</v>
+        <v>4257.153966760719</v>
       </c>
       <c r="G41">
-        <v>287.4350459499174</v>
+        <v>257.1539667607185</v>
       </c>
       <c r="H41">
-        <v>287.4350459499174</v>
+        <v>257.1539667607185</v>
       </c>
       <c r="I41">
-        <v>1417519.175673468</v>
+        <v>1519443.667722016</v>
       </c>
       <c r="J41">
-        <v>909.0009675736243</v>
+        <v>928.6524281993526</v>
       </c>
       <c r="K41">
-        <v>7.185876148747934</v>
+        <v>6.428849169017963</v>
       </c>
       <c r="L41">
-        <v>17.94521206394123</v>
+        <v>18.34757429813319</v>
       </c>
       <c r="M41">
-        <v>8.101462681665046</v>
+        <v>8.216645395259905</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -11171,37 +11171,37 @@
         <v>2000</v>
       </c>
       <c r="C42">
-        <v>8860.840520072432</v>
+        <v>8620.727464198924</v>
       </c>
       <c r="D42">
-        <v>48.93188870608211</v>
+        <v>29.5964005893743</v>
       </c>
       <c r="E42">
-        <v>0.404897514678931</v>
+        <v>0.4036028755314049</v>
       </c>
       <c r="F42">
-        <v>3856.996847419526</v>
+        <v>3806.288637024717</v>
       </c>
       <c r="G42">
-        <v>1856.996847419526</v>
+        <v>1806.288637024717</v>
       </c>
       <c r="H42">
-        <v>1856.996847419526</v>
+        <v>1806.288637024717</v>
       </c>
       <c r="I42">
-        <v>1468292.128564783</v>
+        <v>1563024.542035081</v>
       </c>
       <c r="J42">
-        <v>932.7008645697717</v>
+        <v>950.5933334199868</v>
       </c>
       <c r="K42">
-        <v>92.84984237097629</v>
+        <v>90.31443185123582</v>
       </c>
       <c r="L42">
-        <v>19.81782782161711</v>
+        <v>20.14674573696075</v>
       </c>
       <c r="M42">
-        <v>9.886593455735836</v>
+        <v>9.927164438482947</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -11212,37 +11212,37 @@
         <v>5000</v>
       </c>
       <c r="C43">
-        <v>8873.569714700716</v>
+        <v>8610.671754806022</v>
       </c>
       <c r="D43">
-        <v>45.3116192983023</v>
+        <v>25.63118959114668</v>
       </c>
       <c r="E43">
-        <v>0.6060850440506886</v>
+        <v>0.6061965710446221</v>
       </c>
       <c r="F43">
-        <v>5442.266539673964</v>
+        <v>5268.326852447119</v>
       </c>
       <c r="G43">
-        <v>442.266539673964</v>
+        <v>268.3268524471187</v>
       </c>
       <c r="H43">
-        <v>442.266539673964</v>
+        <v>268.3268524471187</v>
       </c>
       <c r="I43">
-        <v>1437250.849626988</v>
+        <v>1526658.072710913</v>
       </c>
       <c r="J43">
-        <v>920.7390517674348</v>
+        <v>933.9526875425998</v>
       </c>
       <c r="K43">
-        <v>8.845330793479279</v>
+        <v>5.366537048942373</v>
       </c>
       <c r="L43">
-        <v>19.55020594288204</v>
+        <v>19.78625284213103</v>
       </c>
       <c r="M43">
-        <v>10.49537410728777</v>
+        <v>10.3913434983186</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -11253,37 +11253,37 @@
         <v>7000</v>
       </c>
       <c r="C44">
-        <v>8885.989733871022</v>
+        <v>8605.415995148254</v>
       </c>
       <c r="D44">
-        <v>42.02245928550265</v>
+        <v>22.54249466625521</v>
       </c>
       <c r="E44">
-        <v>0.8413906766312695</v>
+        <v>0.8410104573713204</v>
       </c>
       <c r="F44">
-        <v>7557.413935345327</v>
+        <v>7289.676241697325</v>
       </c>
       <c r="G44">
-        <v>557.4139353453265</v>
+        <v>289.6762416973252</v>
       </c>
       <c r="H44">
-        <v>557.4139353453265</v>
+        <v>289.6762416973252</v>
       </c>
       <c r="I44">
-        <v>1410428.455476754</v>
+        <v>1492306.983479793</v>
       </c>
       <c r="J44">
-        <v>912.0884537573847</v>
+        <v>918.6127721653313</v>
       </c>
       <c r="K44">
-        <v>7.96305621921895</v>
+        <v>4.138232024247503</v>
       </c>
       <c r="L44">
-        <v>19.27432142565197</v>
+        <v>19.41368091789571</v>
       </c>
       <c r="M44">
-        <v>11.20605649235936</v>
+        <v>10.88020952024327</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -11294,37 +11294,37 @@
         <v>10000</v>
       </c>
       <c r="C45">
-        <v>9087.301611222436</v>
+        <v>8942.92154041765</v>
       </c>
       <c r="D45">
-        <v>57.95140109209382</v>
+        <v>54.03879972656928</v>
       </c>
       <c r="E45">
-        <v>0.8529979503905568</v>
+        <v>0.8539323752454463</v>
       </c>
       <c r="F45">
-        <v>7370.116548483676</v>
+        <v>7114.347048403553</v>
       </c>
       <c r="G45">
-        <v>-2629.883451516324</v>
+        <v>-2885.652951596447</v>
       </c>
       <c r="H45">
-        <v>2629.883451516324</v>
+        <v>2885.652951596447</v>
       </c>
       <c r="I45">
-        <v>1538471.676711234</v>
+        <v>1651253.168911828</v>
       </c>
       <c r="J45">
-        <v>952.0371746354996</v>
+        <v>964.3578926172178</v>
       </c>
       <c r="K45">
-        <v>26.29883451516324</v>
+        <v>28.85652951596447</v>
       </c>
       <c r="L45">
-        <v>19.43768219517549</v>
+        <v>19.63328204808336</v>
       </c>
       <c r="M45">
-        <v>7.973461005053673</v>
+        <v>7.371792704719061</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -11335,37 +11335,37 @@
         <v>14000</v>
       </c>
       <c r="C46">
-        <v>9311.462218791565</v>
+        <v>9309.955421467181</v>
       </c>
       <c r="D46">
-        <v>74.57232173979733</v>
+        <v>85.33830785886541</v>
       </c>
       <c r="E46">
-        <v>1.16082295531281</v>
+        <v>1.160422328333643</v>
       </c>
       <c r="F46">
-        <v>10267.78841064468</v>
+        <v>10097.04535636308</v>
       </c>
       <c r="G46">
-        <v>-3732.211589355318</v>
+        <v>-3902.95464363692</v>
       </c>
       <c r="H46">
-        <v>3732.211589355318</v>
+        <v>3902.95464363692</v>
       </c>
       <c r="I46">
-        <v>1820083.76014321</v>
+        <v>1959930.4821249</v>
       </c>
       <c r="J46">
-        <v>1015.222956788223</v>
+        <v>1031.14418241312</v>
       </c>
       <c r="K46">
-        <v>26.65865420968084</v>
+        <v>27.87824745454943</v>
       </c>
       <c r="L46">
-        <v>19.60179519550516</v>
+        <v>19.82066762550304</v>
       </c>
       <c r="M46">
-        <v>3.8009578803952</v>
+        <v>3.109256579806253</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -11376,37 +11376,37 @@
         <v>16000</v>
       </c>
       <c r="C47">
-        <v>9387.933907641833</v>
+        <v>9397.706845256962</v>
       </c>
       <c r="D47">
-        <v>74.7622584508444</v>
+        <v>85.579619451957</v>
       </c>
       <c r="E47">
-        <v>1.6984415707223</v>
+        <v>1.698575017573714</v>
       </c>
       <c r="F47">
-        <v>15935.50551103197</v>
+        <v>15954.46894973744</v>
       </c>
       <c r="G47">
-        <v>-64.49448896802824</v>
+        <v>-45.53105026256162</v>
       </c>
       <c r="H47">
-        <v>64.49448896802824</v>
+        <v>45.53105026256162</v>
       </c>
       <c r="I47">
-        <v>1779729.888564633</v>
+        <v>1916422.539778525</v>
       </c>
       <c r="J47">
-        <v>994.0956575033296</v>
+        <v>1009.24166836533</v>
       </c>
       <c r="K47">
-        <v>0.4030905560501764</v>
+        <v>0.2845690641410101</v>
       </c>
       <c r="L47">
-        <v>19.17515731462838</v>
+        <v>19.38653210191722</v>
       </c>
       <c r="M47">
-        <v>3.816861265166098</v>
+        <v>3.131619395732577</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -11417,37 +11417,37 @@
         <v>16000</v>
       </c>
       <c r="C48">
-        <v>9446.297274703798</v>
+        <v>9451.306484863302</v>
       </c>
       <c r="D48">
-        <v>73.12236931195652</v>
+        <v>82.38162146739532</v>
       </c>
       <c r="E48">
-        <v>1.745781821111605</v>
+        <v>1.746860366989314</v>
       </c>
       <c r="F48">
-        <v>16574.4725836187</v>
+        <v>16622.84824746861</v>
       </c>
       <c r="G48">
-        <v>574.4725836187026</v>
+        <v>622.8482474686134</v>
       </c>
       <c r="H48">
-        <v>574.4725836187026</v>
+        <v>622.8482474686134</v>
       </c>
       <c r="I48">
-        <v>1748214.429016044</v>
+        <v>1883194.657161051</v>
       </c>
       <c r="J48">
-        <v>984.9734167667073</v>
+        <v>1000.841811389314</v>
       </c>
       <c r="K48">
-        <v>3.590453647616892</v>
+        <v>3.892801546678834</v>
       </c>
       <c r="L48">
-        <v>18.83635940882378</v>
+        <v>19.04971187245551</v>
       </c>
       <c r="M48">
-        <v>4.435447412331274</v>
+        <v>3.780226793134333</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -11458,37 +11458,37 @@
         <v>20000</v>
       </c>
       <c r="C49">
-        <v>9518.785488376388</v>
+        <v>9530.261597302815</v>
       </c>
       <c r="D49">
-        <v>73.05895374801987</v>
+        <v>82.03897056460708</v>
       </c>
       <c r="E49">
-        <v>2.103505058525819</v>
+        <v>2.105469488238644</v>
       </c>
       <c r="F49">
-        <v>20026.68236938233</v>
+        <v>20080.18926502265</v>
       </c>
       <c r="G49">
-        <v>26.68236938233167</v>
+        <v>80.18926502265458</v>
       </c>
       <c r="H49">
-        <v>26.68236938233167</v>
+        <v>80.18926502265458</v>
       </c>
       <c r="I49">
-        <v>1711033.525182423</v>
+        <v>1843263.501013473</v>
       </c>
       <c r="J49">
-        <v>964.5842455457631</v>
+        <v>981.2534593389598</v>
       </c>
       <c r="K49">
-        <v>0.1334118469116584</v>
+        <v>0.4009463251132729</v>
       </c>
       <c r="L49">
-        <v>18.43842435431501</v>
+        <v>18.65292962676738</v>
       </c>
       <c r="M49">
-        <v>4.556864972958737</v>
+        <v>3.937411134049328</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -11499,37 +11499,37 @@
         <v>12000</v>
       </c>
       <c r="C50">
-        <v>9659.691257690418</v>
+        <v>9731.626985935232</v>
       </c>
       <c r="D50">
-        <v>79.84363530462082</v>
+        <v>93.97161237138812</v>
       </c>
       <c r="E50">
-        <v>1.110638776422225</v>
+        <v>1.110679212905241</v>
       </c>
       <c r="F50">
-        <v>10512.78091117865</v>
+        <v>10545.44053849322</v>
       </c>
       <c r="G50">
-        <v>-1487.219088821346</v>
+        <v>-1454.55946150678</v>
       </c>
       <c r="H50">
-        <v>1487.219088821346</v>
+        <v>1454.55946150678</v>
       </c>
       <c r="I50">
-        <v>1721466.589619343</v>
+        <v>1848940.161972752</v>
       </c>
       <c r="J50">
-        <v>975.4724714473377</v>
+        <v>991.1140010507894</v>
       </c>
       <c r="K50">
-        <v>12.39349240684455</v>
+        <v>12.12132884588983</v>
       </c>
       <c r="L50">
-        <v>18.31248827207604</v>
+        <v>18.5168546104991</v>
       </c>
       <c r="M50">
-        <v>2.981387131160036</v>
+        <v>2.430637476682572</v>
       </c>
     </row>
     <row r="51" spans="1:13">
@@ -11540,37 +11540,37 @@
         <v>5000</v>
       </c>
       <c r="C51">
-        <v>9851.244147409778</v>
+        <v>10017.64449379446</v>
       </c>
       <c r="D51">
-        <v>91.01456074609473</v>
+        <v>113.1762019201724</v>
       </c>
       <c r="E51">
-        <v>0.4265780635580081</v>
+        <v>0.4261836724039574</v>
       </c>
       <c r="F51">
-        <v>4067.046376654063</v>
+        <v>4107.883417829801</v>
       </c>
       <c r="G51">
-        <v>-932.9536233459371</v>
+        <v>-892.1165821701989</v>
       </c>
       <c r="H51">
-        <v>932.9536233459371</v>
+        <v>892.1165821701989</v>
       </c>
       <c r="I51">
-        <v>1704097.933980465</v>
+        <v>1827448.974915819</v>
       </c>
       <c r="J51">
-        <v>974.6047398534316</v>
+        <v>989.0936455634305</v>
       </c>
       <c r="K51">
-        <v>18.65907246691874</v>
+        <v>17.84233164340398</v>
       </c>
       <c r="L51">
-        <v>18.31956141890957</v>
+        <v>18.50308883566042</v>
       </c>
       <c r="M51">
-        <v>2.026778004511955</v>
+        <v>1.533648769510147</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -11581,37 +11581,37 @@
         <v>2000</v>
       </c>
       <c r="C52">
-        <v>9648.07774582526</v>
+        <v>9584.17791410238</v>
       </c>
       <c r="D52">
-        <v>61.59646451303345</v>
+        <v>58.51192375894681</v>
       </c>
       <c r="E52">
-        <v>0.4642278914104774</v>
+        <v>0.4645440068768968</v>
       </c>
       <c r="F52">
-        <v>4899.306184922589</v>
+        <v>4994.227607861023</v>
       </c>
       <c r="G52">
-        <v>2899.306184922589</v>
+        <v>2994.227607861023</v>
       </c>
       <c r="H52">
-        <v>2899.306184922589</v>
+        <v>2994.227607861023</v>
       </c>
       <c r="I52">
-        <v>1838135.502379463</v>
+        <v>1970207.974771045</v>
       </c>
       <c r="J52">
-        <v>1013.098768754815</v>
+        <v>1029.196324809382</v>
       </c>
       <c r="K52">
-        <v>144.9653092461294</v>
+        <v>149.7113803930511</v>
       </c>
       <c r="L52">
-        <v>20.85247637545396</v>
+        <v>21.12725466680823</v>
       </c>
       <c r="M52">
-        <v>4.811587759347431</v>
+        <v>4.383177195220935</v>
       </c>
     </row>
     <row r="53" spans="1:13">
@@ -11622,37 +11622,37 @@
         <v>3000</v>
       </c>
       <c r="C53">
-        <v>9542.459582480902</v>
+        <v>9347.93996200639</v>
       </c>
       <c r="D53">
-        <v>44.87500172729435</v>
+        <v>29.03693617345319</v>
       </c>
       <c r="E53">
-        <v>0.4556078171714346</v>
+        <v>0.4561081675870187</v>
       </c>
       <c r="F53">
-        <v>4576.162784585688</v>
+        <v>4542.944770188278</v>
       </c>
       <c r="G53">
-        <v>1576.162784585688</v>
+        <v>1542.944770188278</v>
       </c>
       <c r="H53">
-        <v>1576.162784585688</v>
+        <v>1542.944770188278</v>
       </c>
       <c r="I53">
-        <v>1850805.181225217</v>
+        <v>1978256.417694189</v>
       </c>
       <c r="J53">
-        <v>1024.139239653459</v>
+        <v>1039.26982373838</v>
       </c>
       <c r="K53">
-        <v>52.53875948618961</v>
+        <v>51.43149233960928</v>
       </c>
       <c r="L53">
-        <v>21.47377604429191</v>
+        <v>21.72145540549061</v>
       </c>
       <c r="M53">
-        <v>6.29872986950395</v>
+        <v>5.825334761208254</v>
       </c>
     </row>
     <row r="54" spans="1:13">
@@ -11663,37 +11663,37 @@
         <v>2000</v>
       </c>
       <c r="C54">
-        <v>9354.943932584471</v>
+        <v>8979.031924722321</v>
       </c>
       <c r="D54">
-        <v>21.63593656492176</v>
+        <v>-10.75756117229903</v>
       </c>
       <c r="E54">
-        <v>0.385786833084816</v>
+        <v>0.385516704127616</v>
       </c>
       <c r="F54">
-        <v>3881.887945541261</v>
+        <v>3784.574839896939</v>
       </c>
       <c r="G54">
-        <v>1881.887945541261</v>
+        <v>1784.574839896939</v>
       </c>
       <c r="H54">
-        <v>1881.887945541261</v>
+        <v>1784.574839896939</v>
       </c>
       <c r="I54">
-        <v>1883318.586193454</v>
+        <v>2001457.3973384</v>
       </c>
       <c r="J54">
-        <v>1040.634407074378</v>
+        <v>1053.60261251066</v>
       </c>
       <c r="K54">
-        <v>94.09439727706304</v>
+        <v>89.22874199484697</v>
       </c>
       <c r="L54">
-        <v>22.87032645261444</v>
+        <v>23.01967245528592</v>
       </c>
       <c r="M54">
-        <v>8.007292770862609</v>
+        <v>7.439872848944355</v>
       </c>
     </row>
     <row r="55" spans="1:13">
@@ -11704,37 +11704,37 @@
         <v>7000</v>
       </c>
       <c r="C55">
-        <v>9485.227590281054</v>
+        <v>9200.396519394773</v>
       </c>
       <c r="D55">
-        <v>32.50070867808796</v>
+        <v>12.45465441217606</v>
       </c>
       <c r="E55">
-        <v>0.6192755068646297</v>
+        <v>0.6216605912604118</v>
       </c>
       <c r="F55">
-        <v>5683.00482303821</v>
+        <v>5436.537167371414</v>
       </c>
       <c r="G55">
-        <v>-1316.99517696179</v>
+        <v>-1563.462832628586</v>
       </c>
       <c r="H55">
-        <v>1316.99517696179</v>
+        <v>1563.462832628586</v>
       </c>
       <c r="I55">
-        <v>1880510.241098117</v>
+        <v>2009815.107369959</v>
       </c>
       <c r="J55">
-        <v>1045.848761223198</v>
+        <v>1063.222616663829</v>
       </c>
       <c r="K55">
-        <v>18.81421681373986</v>
+        <v>22.33518332326551</v>
       </c>
       <c r="L55">
-        <v>22.79379608206963</v>
+        <v>23.00675756600252</v>
       </c>
       <c r="M55">
-        <v>6.708110625584556</v>
+        <v>5.902062784797232</v>
       </c>
     </row>
     <row r="56" spans="1:13">
@@ -11745,37 +11745,37 @@
         <v>6000</v>
       </c>
       <c r="C56">
-        <v>9398.394444352272</v>
+        <v>9025.779330924392</v>
       </c>
       <c r="D56">
-        <v>20.56732321740097</v>
+        <v>-6.252529876079716</v>
       </c>
       <c r="E56">
-        <v>0.8210923004343914</v>
+        <v>0.8233856657061511</v>
       </c>
       <c r="F56">
-        <v>8008.127853453815</v>
+        <v>7748.104179377289</v>
       </c>
       <c r="G56">
-        <v>2008.127853453815</v>
+        <v>1748.104179377289</v>
       </c>
       <c r="H56">
-        <v>2008.127853453815</v>
+        <v>1748.104179377289</v>
       </c>
       <c r="I56">
-        <v>1920363.338037356</v>
+        <v>2029186.461343781</v>
       </c>
       <c r="J56">
-        <v>1063.668744412653</v>
+        <v>1075.90560856593</v>
       </c>
       <c r="K56">
-        <v>33.46879755756358</v>
+        <v>29.13506965628815</v>
       </c>
       <c r="L56">
-        <v>22.99148129457878</v>
+        <v>23.12024482693374</v>
       </c>
       <c r="M56">
-        <v>8.483653476489465</v>
+        <v>7.457262749878072</v>
       </c>
     </row>
     <row r="57" spans="1:13">
@@ -11786,37 +11786,37 @@
         <v>8000</v>
       </c>
       <c r="C57">
-        <v>9416.947982980379</v>
+        <v>9050.927490077662</v>
       </c>
       <c r="D57">
-        <v>20.3659447584715</v>
+        <v>-3.112460973144728</v>
       </c>
       <c r="E57">
-        <v>0.8526513696461825</v>
+        <v>0.8569278692489161</v>
       </c>
       <c r="F57">
-        <v>8034.355082543948</v>
+        <v>7702.065944809147</v>
       </c>
       <c r="G57">
-        <v>34.3550825439479</v>
+        <v>-297.9340551908526</v>
       </c>
       <c r="H57">
-        <v>34.3550825439479</v>
+        <v>297.9340551908526</v>
       </c>
       <c r="I57">
-        <v>1885469.100467524</v>
+        <v>1993906.065705575</v>
       </c>
       <c r="J57">
-        <v>1044.953950560495</v>
+        <v>1061.760671231837</v>
       </c>
       <c r="K57">
-        <v>0.4294385317993488</v>
+        <v>3.724175689885658</v>
       </c>
       <c r="L57">
-        <v>22.58126233525552</v>
+        <v>22.76758902444195</v>
       </c>
       <c r="M57">
-        <v>8.668470145555126</v>
+        <v>7.276005762192995</v>
       </c>
     </row>
     <row r="58" spans="1:13">
@@ -11827,37 +11827,37 @@
         <v>10000</v>
       </c>
       <c r="C58">
-        <v>9396.177135972219</v>
+        <v>9009.091375380074</v>
       </c>
       <c r="D58">
-        <v>16.25226558180837</v>
+        <v>-6.984826345589017</v>
       </c>
       <c r="E58">
-        <v>1.15116692075224</v>
+        <v>1.155379080673499</v>
       </c>
       <c r="F58">
-        <v>10955.05064381256</v>
+        <v>10499.28658240559</v>
       </c>
       <c r="G58">
-        <v>955.0506438125594</v>
+        <v>499.286582405588</v>
       </c>
       <c r="H58">
-        <v>955.0506438125594</v>
+        <v>499.286582405588</v>
       </c>
       <c r="I58">
-        <v>1868087.897463582</v>
+        <v>1962752.155449587</v>
       </c>
       <c r="J58">
-        <v>1043.348534368568</v>
+        <v>1051.716491074226</v>
       </c>
       <c r="K58">
-        <v>9.550506438125595</v>
+        <v>4.99286582405588</v>
       </c>
       <c r="L58">
-        <v>22.34857026566392</v>
+        <v>22.45018325300649</v>
       </c>
       <c r="M58">
-        <v>9.597179118851276</v>
+        <v>7.820228563648032</v>
       </c>
     </row>
     <row r="59" spans="1:13">
@@ -11868,37 +11868,37 @@
         <v>20000</v>
       </c>
       <c r="C59">
-        <v>9530.582969274492</v>
+        <v>9251.628765916026</v>
       </c>
       <c r="D59">
-        <v>28.06762235385484</v>
+        <v>17.96739534256508</v>
       </c>
       <c r="E59">
-        <v>1.738448165324734</v>
+        <v>1.744895666778065</v>
       </c>
       <c r="F59">
-        <v>15986.46137708818</v>
+        <v>15290.7532897267</v>
       </c>
       <c r="G59">
-        <v>-4013.538622911818</v>
+        <v>-4709.246710273301</v>
       </c>
       <c r="H59">
-        <v>4013.538622911818</v>
+        <v>4709.246710273301</v>
       </c>
       <c r="I59">
-        <v>2117919.553255535</v>
+        <v>2317388.162866611</v>
       </c>
       <c r="J59">
-        <v>1095.457132413186</v>
+        <v>1115.88368790228</v>
       </c>
       <c r="K59">
-        <v>20.06769311455909</v>
+        <v>23.54623355136651</v>
       </c>
       <c r="L59">
-        <v>22.30855487704804</v>
+        <v>22.46941220560929</v>
       </c>
       <c r="M59">
-        <v>5.476858899624491</v>
+        <v>3.150343241143331</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -11909,37 +11909,37 @@
         <v>20000</v>
       </c>
       <c r="C60">
-        <v>9653.527326015126</v>
+        <v>9465.752587259405</v>
       </c>
       <c r="D60">
-        <v>37.55529579253279</v>
+        <v>37.58303794264647</v>
       </c>
       <c r="E60">
-        <v>1.778381796005318</v>
+        <v>1.783462337404781</v>
       </c>
       <c r="F60">
-        <v>16687.31843722246</v>
+        <v>16192.69015209892</v>
       </c>
       <c r="G60">
-        <v>-3312.681562777543</v>
+        <v>-3807.309847901079</v>
       </c>
       <c r="H60">
-        <v>3312.681562777543</v>
+        <v>3807.309847901079</v>
       </c>
       <c r="I60">
-        <v>2270608.166757444</v>
+        <v>2527357.475195195</v>
       </c>
       <c r="J60">
-        <v>1133.685139833261</v>
+        <v>1162.287587212604</v>
       </c>
       <c r="K60">
-        <v>16.56340781388771</v>
+        <v>19.03654923950539</v>
       </c>
       <c r="L60">
-        <v>22.20950061733838</v>
+        <v>22.41022491309026</v>
       </c>
       <c r="M60">
-        <v>2.370131253931699</v>
+        <v>-0.2511368245066231</v>
       </c>
     </row>
     <row r="61" spans="1:13">
@@ -11950,37 +11950,37 @@
         <v>22000</v>
       </c>
       <c r="C61">
-        <v>9729.465193693832</v>
+        <v>9588.443252464807</v>
       </c>
       <c r="D61">
-        <v>41.39355298115007</v>
+        <v>46.09380066892204</v>
       </c>
       <c r="E61">
-        <v>2.119271811556689</v>
+        <v>2.124365415810222</v>
       </c>
       <c r="F61">
-        <v>20385.24131756407</v>
+        <v>20008.98319535423</v>
       </c>
       <c r="G61">
-        <v>-1614.758682435931</v>
+        <v>-1991.016804645769</v>
       </c>
       <c r="H61">
-        <v>1614.758682435931</v>
+        <v>1991.016804645769</v>
       </c>
       <c r="I61">
-        <v>2276317.275837864</v>
+        <v>2551709.855554291</v>
       </c>
       <c r="J61">
-        <v>1141.838928690934</v>
+        <v>1176.3338451352</v>
       </c>
       <c r="K61">
-        <v>7.339812192890598</v>
+        <v>9.050076384753497</v>
       </c>
       <c r="L61">
-        <v>21.95747199997486</v>
+        <v>22.18378171769472</v>
       </c>
       <c r="M61">
-        <v>0.9390325313484144</v>
+        <v>-1.940699086320538</v>
       </c>
     </row>
     <row r="62" spans="1:13">
@@ -11991,37 +11991,37 @@
         <v>8000</v>
       </c>
       <c r="C62">
-        <v>9642.468910864074</v>
+        <v>9415.680699332477</v>
       </c>
       <c r="D62">
-        <v>28.5545694000593</v>
+        <v>24.20816528879683</v>
       </c>
       <c r="E62">
-        <v>1.082541202057231</v>
+        <v>1.084575940007766</v>
       </c>
       <c r="F62">
-        <v>10851.8946030015</v>
+        <v>10700.88003088095</v>
       </c>
       <c r="G62">
-        <v>2851.894603001496</v>
+        <v>2700.880030880951</v>
       </c>
       <c r="H62">
-        <v>2851.894603001496</v>
+        <v>2700.880030880951</v>
       </c>
       <c r="I62">
-        <v>2373933.701684385</v>
+        <v>2630760.573648578</v>
       </c>
       <c r="J62">
-        <v>1170.33985659611</v>
+        <v>1201.742948230962</v>
       </c>
       <c r="K62">
-        <v>35.6486825375187</v>
+        <v>33.76100038601189</v>
       </c>
       <c r="L62">
-        <v>22.18565884226726</v>
+        <v>22.37673536216667</v>
       </c>
       <c r="M62">
-        <v>3.352973480725042</v>
+        <v>0.347803174576078</v>
       </c>
     </row>
     <row r="63" spans="1:13">
@@ -12029,10 +12029,10 @@
         <v>61</v>
       </c>
       <c r="E63">
-        <v>0.4265780635580081</v>
+        <v>0.4261836724039574</v>
       </c>
       <c r="F63">
-        <v>4150.376421780956</v>
+        <v>4086.437957972398</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -12040,10 +12040,10 @@
         <v>62</v>
       </c>
       <c r="E64">
-        <v>0.4642278914104774</v>
+        <v>0.4645440068768968</v>
       </c>
       <c r="F64">
-        <v>4535.905153238547</v>
+        <v>4475.666447066672</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -12051,10 +12051,10 @@
         <v>63</v>
       </c>
       <c r="E65">
-        <v>0.4556078171714346</v>
+        <v>0.4561081675870187</v>
       </c>
       <c r="F65">
-        <v>4470.538851781719</v>
+        <v>4415.414799814283</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -12062,10 +12062,10 @@
         <v>64</v>
       </c>
       <c r="E66">
-        <v>0.385786833084816</v>
+        <v>0.385516704127616</v>
       </c>
       <c r="F66">
-        <v>3801.406827828269</v>
+        <v>3749.814830748705</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -12073,10 +12073,10 @@
         <v>65</v>
       </c>
       <c r="E67">
-        <v>0.6192755068646297</v>
+        <v>0.6216605912604118</v>
       </c>
       <c r="F67">
-        <v>6127.755543359839</v>
+        <v>6075.376099103305</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -12084,10 +12084,10 @@
         <v>66</v>
       </c>
       <c r="E68">
-        <v>0.8210923004343914</v>
+        <v>0.8233856657061511</v>
       </c>
       <c r="F68">
-        <v>8158.728596088637</v>
+        <v>8084.751604259923</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -12095,10 +12095,10 @@
         <v>67</v>
       </c>
       <c r="E69">
-        <v>0.8526513696461825</v>
+        <v>0.8569278692489161</v>
       </c>
       <c r="F69">
-        <v>8507.607441191301</v>
+        <v>8453.598620105637</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -12106,10 +12106,10 @@
         <v>68</v>
       </c>
       <c r="E70">
-        <v>1.15116692075224</v>
+        <v>1.155379080673499</v>
       </c>
       <c r="F70">
-        <v>11533.79471006076</v>
+        <v>11451.07744141405</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -12117,10 +12117,10 @@
         <v>69</v>
       </c>
       <c r="E71">
-        <v>1.738448165324734</v>
+        <v>1.744895666778065</v>
       </c>
       <c r="F71">
-        <v>17489.85528545872</v>
+        <v>17374.26406679349</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -12128,10 +12128,10 @@
         <v>70</v>
       </c>
       <c r="E72">
-        <v>1.778381796005318</v>
+        <v>1.783462337404781</v>
       </c>
       <c r="F72">
-        <v>17965.2256551754</v>
+        <v>17840.48643244178</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -12139,10 +12139,10 @@
         <v>71</v>
       </c>
       <c r="E73">
-        <v>2.119271811556689</v>
+        <v>2.124365415810222</v>
       </c>
       <c r="F73">
-        <v>21496.62322664858</v>
+        <v>21348.5579972382</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -12150,10 +12150,10 @@
         <v>72</v>
       </c>
       <c r="E74">
-        <v>1.082541202057231</v>
+        <v>1.084575940007766</v>
       </c>
       <c r="F74">
-        <v>11025.45943877329</v>
+        <v>10949.30935283243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>